<commit_message>
added base for opening excel
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murat\Desktop\wew\hepevento\hepevento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cba1c346281a1e0/Documents/Python/hepevento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B8D425-8D1D-42A6-80FF-8EE16EC50679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{86B8D425-8D1D-42A6-80FF-8EE16EC50679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D36FA5FC-24E1-40AB-98C2-6F165F7D6F9F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CE827ABE-3065-49E7-A6B5-80164542B991}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{CE827ABE-3065-49E7-A6B5-80164542B991}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -47,17 +47,37 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Location</t>
+    <t>Aamer</t>
+  </si>
+  <si>
+    <t>aamermurhaf@hotmail.com</t>
+  </si>
+  <si>
+    <t>Number of guests</t>
+  </si>
+  <si>
+    <t>Aya</t>
+  </si>
+  <si>
+    <t>ayashams42@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,13 +100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,36 +423,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539D6A7F-A37A-44F0-AD46-B1438725F76B}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>966535288851</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>905525194276</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{15E003B6-D134-4BF1-9759-C7F26C45C4D5}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{97ADBF7F-14FB-4EC2-AF97-0E5F92EE70AC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>